<commit_message>
replace multiple requirements.txt with single one
</commit_message>
<xml_diff>
--- a/Sprint2Vec_Config.xlsx
+++ b/Sprint2Vec_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peerachaibanyongrakkul/Documents/GitHub/sprint2vec_revision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977BB0FD-3D35-B244-A450-BBECEB11E897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AEAE01-5020-4E4B-9A19-8115008A4EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="27040" windowHeight="15900" firstSheet="3" activeTab="10" xr2:uid="{FFD04613-4062-8743-BE5A-040E02029004}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15860" xr2:uid="{FFD04613-4062-8743-BE5A-040E02029004}"/>
   </bookViews>
   <sheets>
     <sheet name="Apache_Productivity" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -316,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,13 +345,16 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF9BC59-29F9-2C45-AF69-9EA446588202}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,12 +929,12 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="K15" s="9"/>
+      <c r="K15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="K3:K8"/>
-    <mergeCell ref="K10:K15"/>
+    <mergeCell ref="K10:K14"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="I3:I8"/>
@@ -1137,7 +1140,7 @@
       <c r="I10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>102392</v>
       </c>
     </row>
@@ -1148,7 +1151,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1166,7 +1169,7 @@
         <v>41</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1184,7 +1187,7 @@
         <v>41</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1202,7 +1205,7 @@
         <v>41</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1217,7 +1220,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1239,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFCEBED-0CEF-FC48-A0B3-6AC023E7484D}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,24 +1283,24 @@
       <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="13">
         <f>1.90287280082702+5.26696062088012</f>
         <v>7.16983342170714</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="13">
         <v>14548.182986736199</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="13">
         <v>194.45071220397901</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="13">
         <v>12874.4389959573</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="13">
         <f>(0.0492518510742885+0.0694238417364465)/2</f>
         <v>5.9337846405367503E-2</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="13">
         <f>SUM(B2:F2)</f>
         <v>27624.301866165588</v>
       </c>
@@ -1306,24 +1309,24 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="13">
         <f>1.93603992462158+1.42025876045227</f>
         <v>3.3562986850738499</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="13">
         <v>5390.3550209999003</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="13">
         <v>261.33614730834898</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="13">
         <v>25772.546979665702</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="13">
         <f>(0.0558837963766595+0.0648584602185454)/2</f>
         <v>6.0371128297602453E-2</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="13">
         <f t="shared" ref="G3:G6" si="0">SUM(B3:F3)</f>
         <v>31427.654817787319</v>
       </c>
@@ -1332,24 +1335,24 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <f>3.61102843284606+4.88808369636535</f>
         <v>8.4991121292114098</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>24119.2870918802</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <v>1286.2566804885801</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <v>11494.557356953601</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="13">
         <f>(0.06578396210925+0.0784751268545021)/2</f>
         <v>7.2129544481876057E-2</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="13">
         <f t="shared" si="0"/>
         <v>36908.672370996072</v>
       </c>
@@ -1358,24 +1361,24 @@
       <c r="A5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="13">
         <f>2.31647539138793+7.68053865432739</f>
         <v>9.9970140457153196</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="13">
         <v>23340.2372409296</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="13">
         <v>429.469917297363</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="13">
         <v>12316.5500522932</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="13">
         <f>(0.0505508941214415+0.038844702083911)/2</f>
         <v>4.4697798102676253E-2</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="13">
         <f t="shared" si="0"/>
         <v>36096.298922363982</v>
       </c>
@@ -1384,24 +1387,24 @@
       <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <f>2.15141057968139+4.345960855484</f>
         <v>6.4973714351653893</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>15712.037625675201</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="13">
         <v>269.76839447021399</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="13">
         <v>14927.893893480301</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="13">
         <f>(0.0452411405412508+0.0350504280713148)/2</f>
         <v>4.0145784306282802E-2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="13">
         <f t="shared" si="0"/>
         <v>30916.237430845187</v>
       </c>
@@ -1417,7 +1420,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1427,7 +1430,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1446,7 +1449,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,7 +1928,7 @@
       <c r="I10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>363704</v>
       </c>
     </row>
@@ -1936,7 +1939,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1954,7 +1957,7 @@
         <v>0.25</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1972,7 +1975,7 @@
         <v>0.25</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1990,7 +1993,7 @@
         <v>31</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -2005,7 +2008,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2216,7 +2219,7 @@
       <c r="I10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>257272</v>
       </c>
     </row>
@@ -2227,7 +2230,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -2242,7 +2245,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -2257,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -2272,7 +2275,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -2287,7 +2290,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2495,7 +2498,7 @@
       <c r="I10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>291332</v>
       </c>
     </row>
@@ -2506,7 +2509,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -2524,7 +2527,7 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -2542,7 +2545,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -2560,7 +2563,7 @@
         <v>28</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -2575,7 +2578,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2783,7 +2786,7 @@
       <c r="I10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>291332</v>
       </c>
     </row>
@@ -2794,7 +2797,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -2812,7 +2815,7 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -2830,7 +2833,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -2848,7 +2851,7 @@
         <v>28</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -2863,7 +2866,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3087,7 +3090,7 @@
       <c r="I11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="11">
         <v>257792</v>
       </c>
     </row>
@@ -3098,7 +3101,7 @@
         <v>23</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -3113,7 +3116,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -3128,7 +3131,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -3143,7 +3146,7 @@
         <v>10</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -3158,7 +3161,7 @@
         <v>25</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3382,7 +3385,7 @@
       <c r="I11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="11">
         <v>242760</v>
       </c>
     </row>
@@ -3393,7 +3396,7 @@
         <v>23</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -3411,7 +3414,7 @@
         <v>0.25</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -3429,7 +3432,7 @@
         <v>0.25</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -3447,7 +3450,7 @@
         <v>31</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -3462,7 +3465,7 @@
         <v>25</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="K16" s="10"/>
+      <c r="K16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3673,7 +3676,7 @@
       <c r="I10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="11">
         <v>257272</v>
       </c>
     </row>
@@ -3684,7 +3687,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -3699,7 +3702,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -3714,7 +3717,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="K13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -3729,7 +3732,7 @@
         <v>10</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -3744,7 +3747,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>